<commit_message>
New Flat_JSON folder updated
</commit_message>
<xml_diff>
--- a/SAM/SAM_comb.xlsx
+++ b/SAM/SAM_comb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzrfl\Documents\GitHub\DOE_CSP_PROJECT\SAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E94F07-1F0B-4961-B9FD-D5CF23D58BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005ADF57-90E4-4E6D-B1BB-7F92F1838870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="645" windowWidth="21030" windowHeight="13200" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
+    <workbookView xWindow="8520" yWindow="1095" windowWidth="20250" windowHeight="13575" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -593,7 +593,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>